<commit_message>
updated scrips and results files
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacko\Documents\courses\IntroAI\Final Project\AdversarialAttacks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9700D224-BE52-45B0-A283-2B0A8F3F48BA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F90F51B-3894-4BDF-A037-C035847EDDE7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,18 +38,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>ChangeBestPixel (Test 29) % Change in Confidence</t>
-  </si>
-  <si>
-    <t>ChangeBest2Pixels (Test 29) % Change in Confidence</t>
-  </si>
-  <si>
-    <t>ChangeBestPixel2Iterations (Test 29) % Change in Confidence</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>testing/yaleB01/image0.jpg</t>
   </si>
   <si>
@@ -197,7 +185,19 @@
     <t>success0</t>
   </si>
   <si>
-    <t>ChangeAllPixels % Change in Confidence</t>
+    <t>Average Change in Confidence</t>
+  </si>
+  <si>
+    <t>Change 1 Best Pixel (Test 29) by 128</t>
+  </si>
+  <si>
+    <t>Change 2 Best Pixels (Test 29) by 128</t>
+  </si>
+  <si>
+    <t>Change 1 Best Pixel - 2 Iterations (Test 29+29) by 128</t>
+  </si>
+  <si>
+    <t>Change All Pixels by 20 to 50 (randomly selected)</t>
   </si>
 </sst>
 </file>
@@ -363,9 +363,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.5768635242987487E-2"/>
+          <c:x val="0.17159359440535049"/>
           <c:y val="7.3739856080819427E-2"/>
-          <c:w val="0.68599479890041482"/>
+          <c:w val="0.39738148225768355"/>
           <c:h val="0.65482038685907296"/>
         </c:manualLayout>
       </c:layout>
@@ -382,7 +382,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ChangeBestPixel (Test 29) % Change in Confidence</c:v>
+                  <c:v>Change 1 Best Pixel (Test 29) by 128</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -431,250 +431,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$A$40</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>testing/yaleB01/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>testing/yaleB02/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>testing/yaleB03/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>testing/yaleB04/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>testing/yaleB05/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>testing/yaleB06/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>testing/yaleB07/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>testing/yaleB08/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>testing/yaleB09/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>testing/yaleB10/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>testing/yaleB11/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>testing/yaleB12/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>testing/yaleB13/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>testing/yaleB15/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>testing/yaleB16/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>testing/yaleB17/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>testing/yaleB18/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>testing/yaleB19/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>testing/yaleB20/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>testing/yaleB21/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>testing/yaleB22/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>testing/yaleB23/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>testing/yaleB24/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>testing/yaleB25/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>testing/yaleB26/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>testing/yaleB27/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>testing/yaleB28/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>testing/yaleB29/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>testing/yaleB30/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>testing/yaleB31/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>testing/yaleB32/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>testing/yaleB33/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>testing/yaleB34/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>testing/yaleB35/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>testing/yaleB36/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>testing/yaleB37/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>testing/yaleB38/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>testing/yaleB39/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Average</c:v>
+                  <c:v>Average Change in Confidence</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$40</c:f>
+              <c:f>Sheet1!$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.14780499</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.13733429</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0807973000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11091848999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5239915999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.43089264999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.20237619000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.9535779999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7951706000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.1529560000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.4636369999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.36042449999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.40293225999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.17687037999999999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.11114834</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.15197858</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.12974574</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.0087360000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.5480218000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.8162665E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.2405736</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.1847450000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.4910090000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.42979299999999998</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.8942552999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.10434584</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.1841046E-4</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.1255888000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.14046863000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.34782400000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.20347956</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.8684179999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.14223652000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.47186266999999998</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8.2976713999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7.1077470000000004E-2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.21616393</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>0.14243206482789472</c:v>
                 </c:pt>
               </c:numCache>
@@ -695,7 +467,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ChangeBest2Pixels (Test 29) % Change in Confidence</c:v>
+                  <c:v>Change 2 Best Pixels (Test 29) by 128</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -744,250 +516,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$A$40</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>testing/yaleB01/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>testing/yaleB02/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>testing/yaleB03/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>testing/yaleB04/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>testing/yaleB05/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>testing/yaleB06/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>testing/yaleB07/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>testing/yaleB08/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>testing/yaleB09/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>testing/yaleB10/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>testing/yaleB11/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>testing/yaleB12/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>testing/yaleB13/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>testing/yaleB15/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>testing/yaleB16/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>testing/yaleB17/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>testing/yaleB18/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>testing/yaleB19/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>testing/yaleB20/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>testing/yaleB21/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>testing/yaleB22/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>testing/yaleB23/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>testing/yaleB24/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>testing/yaleB25/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>testing/yaleB26/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>testing/yaleB27/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>testing/yaleB28/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>testing/yaleB29/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>testing/yaleB30/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>testing/yaleB31/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>testing/yaleB32/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>testing/yaleB33/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>testing/yaleB34/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>testing/yaleB35/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>testing/yaleB36/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>testing/yaleB37/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>testing/yaleB38/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>testing/yaleB39/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Average</c:v>
+                  <c:v>Average Change in Confidence</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$40</c:f>
+              <c:f>Sheet1!$C$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.11134028999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.18651234999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.14859386999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.31359841999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.1632670000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5318967</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.43813734999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.20911813000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.4987308E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.19061637000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.6380440000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.48757004999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.52471226000000004</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.41998725999999997</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.2619995</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.27267682999999998</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.30051133000000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.10568027000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.13867424</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.16035342</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.38649228000000002</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.119902514</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.13312879</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.52237210000000001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.3355843000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.24505432999999999</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5.3731389999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7.6185009999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.13159314</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.39467096000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.36175308</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>6.9945530000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.20617062999999999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.53131293999999996</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.12669335000000001</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.9087159999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.25114693999999999</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>0.22730460644736838</c:v>
                 </c:pt>
               </c:numCache>
@@ -1008,14 +552,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ChangeBestPixel2Iterations (Test 29) % Change in Confidence</c:v>
+                  <c:v>Change 1 Best Pixel - 2 Iterations (Test 29+29) by 128</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFD320"/>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1057,250 +603,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:f>Sheet1!$A$40</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>testing/yaleB01/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>testing/yaleB02/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>testing/yaleB03/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>testing/yaleB04/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>testing/yaleB05/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>testing/yaleB06/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>testing/yaleB07/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>testing/yaleB08/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>testing/yaleB09/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>testing/yaleB10/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>testing/yaleB11/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>testing/yaleB12/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>testing/yaleB13/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>testing/yaleB15/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>testing/yaleB16/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>testing/yaleB17/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>testing/yaleB18/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>testing/yaleB19/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>testing/yaleB20/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>testing/yaleB21/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>testing/yaleB22/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>testing/yaleB23/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>testing/yaleB24/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>testing/yaleB25/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>testing/yaleB26/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>testing/yaleB27/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>testing/yaleB28/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>testing/yaleB29/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>testing/yaleB30/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>testing/yaleB31/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>testing/yaleB32/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>testing/yaleB33/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>testing/yaleB34/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>testing/yaleB35/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>testing/yaleB36/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>testing/yaleB37/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>testing/yaleB38/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>testing/yaleB39/image0.jpg</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Average</c:v>
+                  <c:v>Average Change in Confidence</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$40</c:f>
+              <c:f>Sheet1!$D$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.25098251999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.28101596000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.18852587000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.23951833</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.072382E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.60806780000000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.33985515999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.30988294</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8163696E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.23207620000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.10318937</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.55894935000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.56156919999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.29811862</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.30411068000000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.25499535000000001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.43461564000000003</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.13904010999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.10608745999999999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.8962519999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.35588091999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.11528756499999999</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.109188154</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.59405859999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5.0465919999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.21484342000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>6.0360413000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.5239499999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.18396860000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.47567323</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.38969398</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5.4420549999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.21038997000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.68445045000000004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.14526759</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.17478943999999999</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.36577929999999997</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>0.25232126836842095</c:v>
                 </c:pt>
               </c:numCache>
@@ -1321,133 +639,30 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ChangeAllPixels % Change in Confidence</c:v>
+                  <c:v>Change All Pixels by 20 to 50 (randomly selected)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Change in Confidence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$40</c:f>
+              <c:f>Sheet1!$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.91109680000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.59697217000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.87879675999999995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.99791160000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.35594130000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.97999340000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.98694249999999994</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.83760369999999995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.93953679999999995</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.70322879999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.96363469999999996</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.85810149999999996</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.78860145999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.91346585999999996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.93029576999999997</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.94109493</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.65979690000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.87602729999999995</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.99864200000000003</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.99233245999999997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.69709969999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.99611360000000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.65887669999999998</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.76155209999999995</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.97230479999999997</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.97351896999999998</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.57683026999999998</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.9551984</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.8114633</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.67279374999999997</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.93795879999999998</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.92445564000000002</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.69456923000000004</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.92421509999999996</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.36385304000000002</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.94107370000000001</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.95199590000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.99325830000000004</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>0.8399249476315791</c:v>
                 </c:pt>
               </c:numCache>
@@ -1549,8 +764,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.7997399450207445E-2"/>
-              <c:y val="0.1621869587604737"/>
+              <c:x val="2.1011376742464154E-2"/>
+              <c:y val="9.6076964805286616E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1597,10 +812,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79384639921318978"/>
-          <c:y val="0.2103511593962373"/>
-          <c:w val="0.20615360078681028"/>
-          <c:h val="0.39554752694761119"/>
+          <c:x val="0.60584463539015809"/>
+          <c:y val="8.475712430039932E-2"/>
+          <c:w val="0.39415519828082318"/>
+          <c:h val="0.61618556590813112"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1643,20 +858,479 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5768635242987487E-2"/>
+          <c:y val="0.10076193758963031"/>
+          <c:w val="0.88713868639008675"/>
+          <c:h val="0.62779827484222939"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Change All Pixels by 20 to 50 (randomly selected)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>testing/yaleB01/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>testing/yaleB02/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>testing/yaleB03/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>testing/yaleB04/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>testing/yaleB05/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>testing/yaleB06/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>testing/yaleB07/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>testing/yaleB08/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>testing/yaleB09/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>testing/yaleB10/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>testing/yaleB11/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>testing/yaleB12/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>testing/yaleB13/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>testing/yaleB15/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>testing/yaleB16/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>testing/yaleB17/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>testing/yaleB18/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>testing/yaleB19/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>testing/yaleB20/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>testing/yaleB21/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>testing/yaleB22/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>testing/yaleB23/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>testing/yaleB24/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>testing/yaleB25/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>testing/yaleB26/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>testing/yaleB27/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>testing/yaleB28/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>testing/yaleB29/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>testing/yaleB30/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>testing/yaleB31/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>testing/yaleB32/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>testing/yaleB33/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>testing/yaleB34/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>testing/yaleB35/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>testing/yaleB36/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>testing/yaleB37/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>testing/yaleB38/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>testing/yaleB39/image0.jpg</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Average Change in Confidence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>0.91109680000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59697217000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87879675999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99791160000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35594130000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97999340000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98694249999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83760369999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93953679999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70322879999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96363469999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85810149999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.78860145999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91346585999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.93029576999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.94109493</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.65979690000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.87602729999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99864200000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99233245999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.69709969999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99611360000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.65887669999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.76155209999999995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.97230479999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.97351896999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.57683026999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9551984</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.8114633</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.67279374999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.93795879999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.92445564000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.69456923000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.92421509999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.36385304000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.94107370000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.95199590000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.99325830000000004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8399249476315791</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-275E-4B38-B9B1-204608B3A2A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="84491228"/>
+        <c:axId val="81167459"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="84491228"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="81167459"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="81167459"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent Decrease</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in Classifier Confidence</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7997399450207445E-2"/>
+              <c:y val="0.1621869587604737"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84491228"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>198960</xdr:colOff>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>441960</xdr:rowOff>
+      <xdr:rowOff>449580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>21180</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1676,6 +1350,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1074420</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>463980</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>5940</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A61E7F23-BEA4-4FB3-BD78-0FEEA529D493}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1981,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,13 +1713,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>54</v>
@@ -2015,7 +1727,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>0.14780499</v>
@@ -2032,7 +1744,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2">
         <v>0.13733429</v>
@@ -2049,7 +1761,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>6.0807973000000001E-2</v>
@@ -2066,7 +1778,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>0.11091848999999999</v>
@@ -2083,7 +1795,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>1.5239915999999999E-2</v>
@@ -2100,7 +1812,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>0.43089264999999999</v>
@@ -2117,7 +1829,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>0.20237619000000001</v>
@@ -2134,7 +1846,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>8.9535779999999995E-2</v>
@@ -2151,7 +1863,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>1.7951706000000001E-2</v>
@@ -2168,7 +1880,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>7.1529560000000006E-2</v>
@@ -2185,7 +1897,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -2202,7 +1914,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>1.4636369999999999E-2</v>
@@ -2219,7 +1931,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>0.36042449999999998</v>
@@ -2236,7 +1948,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>0.40293225999999999</v>
@@ -2253,7 +1965,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>0.17687037999999999</v>
@@ -2270,7 +1982,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>0.11114834</v>
@@ -2287,7 +1999,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>0.15197858</v>
@@ -2304,7 +2016,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>0.12974574</v>
@@ -2321,7 +2033,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>9.0087360000000005E-2</v>
@@ -2338,7 +2050,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>4.5480218000000003E-2</v>
@@ -2355,7 +2067,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>4.8162665E-2</v>
@@ -2372,7 +2084,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>0.2405736</v>
@@ -2389,7 +2101,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>4.1847450000000001E-2</v>
@@ -2406,7 +2118,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>1.4910090000000001E-2</v>
@@ -2423,7 +2135,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>0.42979299999999998</v>
@@ -2440,7 +2152,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>2.8942552999999999E-2</v>
@@ -2457,7 +2169,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>0.10434584</v>
@@ -2474,7 +2186,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>1.1841046E-4</v>
@@ -2491,7 +2203,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>2.1255888000000001E-2</v>
@@ -2508,7 +2220,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2">
         <v>0.14046863000000001</v>
@@ -2525,7 +2237,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>0.34782400000000002</v>
@@ -2542,7 +2254,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2">
         <v>0.20347956</v>
@@ -2559,7 +2271,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2">
         <v>3.8684179999999999E-2</v>
@@ -2576,7 +2288,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2">
         <v>0.14223652000000001</v>
@@ -2593,7 +2305,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2">
         <v>0.47186266999999998</v>
@@ -2610,7 +2322,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2">
         <v>8.2976713999999993E-2</v>
@@ -2627,7 +2339,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2">
         <v>7.1077470000000004E-2</v>
@@ -2644,7 +2356,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2">
         <v>0.21616393</v>
@@ -2661,7 +2373,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B40" s="2">
         <f>AVERAGE(B1:B39)</f>
@@ -2678,6 +2390,24 @@
       <c r="E40" s="2">
         <f>AVERAGE(E1:E39)</f>
         <v>0.8399249476315791</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <f>STDEV(B2:B39)</f>
+        <v>0.13321151394550365</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42:E42" si="0">STDEV(C2:C39)</f>
+        <v>0.16342673706848609</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>0.18298053129231781</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>0.16983053627859168</v>
       </c>
     </row>
   </sheetData>
@@ -2691,7 +2421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B7B863-F41C-4E21-9C12-0AEC62BF9231}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -2702,30 +2432,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>-0.18656461999999999</v>
@@ -2748,7 +2478,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>-0.23835695000000001</v>
@@ -2771,7 +2501,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>-0.16136903</v>
@@ -2794,7 +2524,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>-0.12413961</v>
@@ -2817,7 +2547,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>-2.0113707000000002E-2</v>
@@ -2840,7 +2570,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>-0.32083869999999998</v>
@@ -2863,7 +2593,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>-0.28227192000000001</v>
@@ -2886,7 +2616,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>-0.17822155000000001</v>
@@ -2909,7 +2639,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>-1.5076041E-2</v>
@@ -2932,7 +2662,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>-9.6608910000000006E-2</v>
@@ -2955,7 +2685,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2978,7 +2708,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>-8.6920140000000007E-2</v>
@@ -3001,7 +2731,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>-0.40737697</v>
@@ -3024,7 +2754,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>-0.25921835999999998</v>
@@ -3047,7 +2777,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>-0.18431923</v>
@@ -3070,7 +2800,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>-0.17754750999999999</v>
@@ -3093,7 +2823,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>-0.13676073999999999</v>
@@ -3116,7 +2846,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>-0.23075065</v>
@@ -3139,7 +2869,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>-0.11064875</v>
@@ -3162,7 +2892,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>-8.0310049999999994E-2</v>
@@ -3185,7 +2915,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>-9.1924309999999995E-2</v>
@@ -3208,7 +2938,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>-0.13531604</v>
@@ -3231,7 +2961,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>-8.2985160000000002E-2</v>
@@ -3254,7 +2984,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>-4.9922139999999997E-2</v>
@@ -3277,7 +3007,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>-0.23236212000000001</v>
@@ -3300,7 +3030,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>-4.8110604000000001E-2</v>
@@ -3323,7 +3053,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>-0.16536313</v>
@@ -3346,7 +3076,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>-4.7641813999999998E-2</v>
@@ -3369,7 +3099,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>-5.334854E-2</v>
@@ -3392,7 +3122,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>-0.12616347999999999</v>
@@ -3415,7 +3145,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>-0.21214947000000001</v>
@@ -3438,7 +3168,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>-0.15091607000000001</v>
@@ -3461,7 +3191,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>-5.0729096000000001E-2</v>
@@ -3484,7 +3214,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>-0.13143157999999999</v>
@@ -3507,7 +3237,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>-0.34313791999999999</v>
@@ -3530,7 +3260,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>-0.12728858000000001</v>
@@ -3553,7 +3283,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>-0.14552593</v>
@@ -3576,7 +3306,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>-0.22942114</v>
@@ -3606,7 +3336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63799EE4-50F1-424F-ADD4-48FF2DAE7ADD}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -3620,21 +3350,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>-8.2763374000000001E-2</v>
@@ -3648,7 +3378,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>-0.15819925000000001</v>
@@ -3662,7 +3392,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>-0.12718916</v>
@@ -3676,7 +3406,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>-0.16253448000000001</v>
@@ -3690,7 +3420,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>-3.0701399000000001E-2</v>
@@ -3704,7 +3434,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>-0.28064802</v>
@@ -3718,7 +3448,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>-0.36390169999999999</v>
@@ -3732,7 +3462,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>-0.12026915000000001</v>
@@ -3746,7 +3476,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>-1.2439609000000001E-2</v>
@@ -3760,7 +3490,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3774,7 +3504,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>-0.11804652</v>
@@ -3788,7 +3518,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>-3.9067923999999997E-2</v>
@@ -3802,7 +3532,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>-0.35535386000000002</v>
@@ -3816,7 +3546,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>-0.24220535000000001</v>
@@ -3830,7 +3560,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>-0.25966755000000002</v>
@@ -3844,7 +3574,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>-0.15296193999999999</v>
@@ -3858,7 +3588,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>-0.14624377999999999</v>
@@ -3872,7 +3602,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>-0.15955059999999999</v>
@@ -3886,7 +3616,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>-8.4100839999999996E-2</v>
@@ -3900,7 +3630,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>-0.1049788</v>
@@ -3914,7 +3644,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>-0.14894909000000001</v>
@@ -3928,7 +3658,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>-0.14695536000000001</v>
@@ -3942,7 +3672,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>-8.6307049999999996E-2</v>
@@ -3956,7 +3686,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>-6.0868084000000003E-2</v>
@@ -3970,7 +3700,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>-0.20432243</v>
@@ -3984,7 +3714,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>-3.1799078000000001E-2</v>
@@ -3998,7 +3728,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>-0.18861622</v>
@@ -4012,7 +3742,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>-4.2409599999999999E-2</v>
@@ -4026,7 +3756,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>-7.3577050000000005E-2</v>
@@ -4040,7 +3770,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>-9.0245010000000001E-2</v>
@@ -4054,7 +3784,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>-0.17602259000000001</v>
@@ -4068,7 +3798,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>-0.14009543999999999</v>
@@ -4082,7 +3812,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>-6.5200984000000003E-2</v>
@@ -4096,7 +3826,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>-0.12879573999999999</v>
@@ -4110,7 +3840,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>-0.26636495999999998</v>
@@ -4124,7 +3854,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>-0.11101317400000001</v>
@@ -4138,7 +3868,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>-8.2497835000000005E-2</v>
@@ -4152,7 +3882,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>-0.15752235000000001</v>

</xml_diff>